<commit_message>
[IMP] clodoo: full python3 functionalities
</commit_message>
<xml_diff>
--- a/clodoo/build/lib/clodoo/transodoo.xlsx
+++ b/clodoo/build/lib/clodoo/transodoo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="784">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -757,21 +757,21 @@
     <t xml:space="preserve">product.product_uom_kgm</t>
   </si>
   <si>
+    <t xml:space="preserve">uom.product_uom_kgm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product.product_uom_ton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uom.product_uom_ton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product.product_uom_unit</t>
+  </si>
+  <si>
     <t xml:space="preserve">uom.product_uom_unit</t>
   </si>
   <si>
-    <t xml:space="preserve">product.product_uom_ton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uom.product_uom_kgm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">product.product_uom_unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uom.product_uom_ton</t>
-  </si>
-  <si>
     <t xml:space="preserve">account.data_account_type_asset</t>
   </si>
   <si>
@@ -2294,6 +2294,9 @@
   </si>
   <si>
     <t xml:space="preserve">zip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notify_email</t>
   </si>
   <si>
     <t xml:space="preserve">res.users</t>
@@ -2378,7 +2381,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2436,6 +2439,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2479,7 +2489,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2501,6 +2511,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2583,13 +2597,13 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="630" topLeftCell="N117" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A144" activeCellId="0" sqref="A144"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="630" topLeftCell="N112" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="J136" activeCellId="0" sqref="J136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="27.30078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="27.31640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.3"/>
@@ -9355,115 +9369,136 @@
         <v>757</v>
       </c>
     </row>
-    <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A449" s="1" t="s">
+    <row r="449" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A449" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B449" s="4"/>
+      <c r="C449" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D449" s="4" t="s">
         <v>758</v>
       </c>
-      <c r="C449" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D449" s="2" t="s">
-        <v>759</v>
-      </c>
-      <c r="E449" s="1" t="s">
-        <v>760</v>
-      </c>
+      <c r="E449" s="4"/>
+      <c r="F449" s="4"/>
+      <c r="G449" s="4"/>
+      <c r="H449" s="4"/>
+      <c r="I449" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="J449" s="4"/>
+      <c r="K449" s="4"/>
+      <c r="L449" s="4"/>
+      <c r="M449" s="4"/>
+      <c r="N449" s="4"/>
+      <c r="O449" s="4"/>
+      <c r="P449" s="4"/>
+      <c r="Q449" s="4"/>
+      <c r="R449" s="4"/>
+      <c r="S449" s="4"/>
+      <c r="T449" s="4"/>
+      <c r="U449" s="4"/>
+      <c r="V449" s="4"/>
+      <c r="W449" s="4"/>
+      <c r="X449" s="4"/>
+      <c r="Y449" s="4"/>
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C450" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D450" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="E450" s="1" t="s">
         <v>761</v>
-      </c>
-      <c r="E450" s="1" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C451" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D451" s="2" t="s">
+        <v>762</v>
+      </c>
       <c r="E451" s="1" t="s">
-        <v>742</v>
+        <v>763</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C452" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E452" s="1" t="s">
-        <v>763</v>
+        <v>742</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="1" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="C453" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D453" s="2" t="s">
+      <c r="E453" s="1" t="s">
         <v>764</v>
-      </c>
-      <c r="E453" s="1" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="C454" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D454" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="E454" s="1" t="s">
         <v>766</v>
-      </c>
-      <c r="C454" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D454" s="2" t="s">
-        <v>767</v>
-      </c>
-      <c r="G454" s="1" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="C455" s="1" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="D455" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H455" s="2" t="s">
-        <v>94</v>
+        <v>768</v>
+      </c>
+      <c r="G455" s="1" t="s">
+        <v>769</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="1" t="s">
-        <v>766</v>
-      </c>
-      <c r="B456" s="2" t="s">
-        <v>123</v>
+        <v>767</v>
       </c>
       <c r="C456" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D456" s="2" t="s">
-        <v>671</v>
+        <v>93</v>
+      </c>
+      <c r="H456" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B457" s="2" t="s">
         <v>123</v>
@@ -9472,12 +9507,12 @@
         <v>34</v>
       </c>
       <c r="D457" s="2" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B458" s="2" t="s">
         <v>123</v>
@@ -9486,12 +9521,12 @@
         <v>34</v>
       </c>
       <c r="D458" s="2" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B459" s="2" t="s">
         <v>123</v>
@@ -9500,15 +9535,12 @@
         <v>34</v>
       </c>
       <c r="D459" s="2" t="s">
-        <v>769</v>
-      </c>
-      <c r="G459" s="1" t="s">
-        <v>102</v>
+        <v>670</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B460" s="2" t="s">
         <v>123</v>
@@ -9525,7 +9557,7 @@
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B461" s="2" t="s">
         <v>123</v>
@@ -9542,7 +9574,7 @@
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B462" s="2" t="s">
         <v>123</v>
@@ -9551,12 +9583,15 @@
         <v>34</v>
       </c>
       <c r="D462" s="2" t="s">
-        <v>677</v>
+        <v>772</v>
+      </c>
+      <c r="G462" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B463" s="2" t="s">
         <v>123</v>
@@ -9565,15 +9600,12 @@
         <v>34</v>
       </c>
       <c r="D463" s="2" t="s">
-        <v>772</v>
-      </c>
-      <c r="G463" s="1" t="s">
-        <v>102</v>
+        <v>677</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="1" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B464" s="2" t="s">
         <v>123</v>
@@ -9590,35 +9622,35 @@
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B465" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C465" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D465" s="2" t="s">
         <v>774</v>
       </c>
-      <c r="C465" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D465" s="2" t="s">
-        <v>775</v>
+      <c r="G465" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A466" s="1" t="s">
-        <v>774</v>
-      </c>
-      <c r="B466" s="2" t="s">
-        <v>123</v>
+        <v>775</v>
       </c>
       <c r="C466" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D466" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="H466" s="2" t="s">
-        <v>670</v>
-      </c>
     </row>
     <row r="467" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A467" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B467" s="2" t="s">
         <v>123</v>
@@ -9627,13 +9659,13 @@
         <v>34</v>
       </c>
       <c r="D467" s="2" t="s">
-        <v>672</v>
+        <v>777</v>
       </c>
       <c r="E467" s="0"/>
       <c r="F467" s="0"/>
       <c r="G467" s="0"/>
       <c r="H467" s="2" t="s">
-        <v>102</v>
+        <v>670</v>
       </c>
       <c r="I467" s="0"/>
       <c r="J467" s="0"/>
@@ -9655,7 +9687,7 @@
     </row>
     <row r="468" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A468" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B468" s="2" t="s">
         <v>123</v>
@@ -9664,12 +9696,14 @@
         <v>34</v>
       </c>
       <c r="D468" s="2" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="E468" s="0"/>
       <c r="F468" s="0"/>
       <c r="G468" s="0"/>
-      <c r="H468" s="0"/>
+      <c r="H468" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="I468" s="0"/>
       <c r="J468" s="0"/>
       <c r="K468" s="0"/>
@@ -9690,7 +9724,7 @@
     </row>
     <row r="469" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A469" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B469" s="2" t="s">
         <v>123</v>
@@ -9699,7 +9733,7 @@
         <v>34</v>
       </c>
       <c r="D469" s="2" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="E469" s="0"/>
       <c r="F469" s="0"/>
@@ -9725,7 +9759,7 @@
     </row>
     <row r="470" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A470" s="1" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B470" s="2" t="s">
         <v>123</v>
@@ -9734,7 +9768,7 @@
         <v>34</v>
       </c>
       <c r="D470" s="2" t="s">
-        <v>670</v>
+        <v>674</v>
       </c>
       <c r="E470" s="0"/>
       <c r="F470" s="0"/>
@@ -9760,14 +9794,16 @@
     </row>
     <row r="471" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A471" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="B471" s="0"/>
+        <v>775</v>
+      </c>
+      <c r="B471" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="C471" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="D471" s="2" t="s">
-        <v>778</v>
+        <v>670</v>
       </c>
       <c r="E471" s="0"/>
       <c r="F471" s="0"/>
@@ -9793,14 +9829,14 @@
     </row>
     <row r="472" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A472" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B472" s="0"/>
       <c r="C472" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D472" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E472" s="0"/>
       <c r="F472" s="0"/>
@@ -9826,20 +9862,18 @@
     </row>
     <row r="473" s="4" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A473" s="1" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B473" s="0"/>
       <c r="C473" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D473" s="2" t="s">
-        <v>591</v>
+        <v>781</v>
       </c>
       <c r="E473" s="0"/>
       <c r="F473" s="0"/>
-      <c r="G473" s="1" t="s">
-        <v>782</v>
-      </c>
+      <c r="G473" s="0"/>
       <c r="H473" s="0"/>
       <c r="I473" s="0"/>
       <c r="J473" s="0"/>
@@ -9859,6 +9893,41 @@
       <c r="X473" s="0"/>
       <c r="Y473" s="0"/>
     </row>
+    <row r="474" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="B474" s="0"/>
+      <c r="C474" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D474" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="E474" s="0"/>
+      <c r="F474" s="0"/>
+      <c r="G474" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="H474" s="0"/>
+      <c r="I474" s="0"/>
+      <c r="J474" s="0"/>
+      <c r="K474" s="0"/>
+      <c r="L474" s="0"/>
+      <c r="M474" s="0"/>
+      <c r="N474" s="0"/>
+      <c r="O474" s="0"/>
+      <c r="P474" s="0"/>
+      <c r="Q474" s="0"/>
+      <c r="R474" s="0"/>
+      <c r="S474" s="0"/>
+      <c r="T474" s="0"/>
+      <c r="U474" s="0"/>
+      <c r="V474" s="0"/>
+      <c r="W474" s="0"/>
+      <c r="X474" s="0"/>
+      <c r="Y474" s="0"/>
+    </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
[IMP] wok_code: new do_migrate command
</commit_message>
<xml_diff>
--- a/clodoo/build/lib/clodoo/transodoo.xlsx
+++ b/clodoo/build/lib/clodoo/transodoo.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2204" uniqueCount="824">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2237" uniqueCount="830">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -2125,12 +2125,33 @@
     <t xml:space="preserve">refunded</t>
   </si>
   <si>
-    <t xml:space="preserve">product_product</t>
+    <t xml:space="preserve">product.product</t>
   </si>
   <si>
     <t xml:space="preserve">name_template</t>
   </si>
   <si>
+    <t xml:space="preserve">image_small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image_512</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image_medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image_1024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image_1920</t>
+  </si>
+  <si>
+    <t xml:space="preserve">product.template</t>
+  </si>
+  <si>
     <t xml:space="preserve">project.task</t>
   </si>
   <si>
@@ -2372,9 +2393,6 @@
   </si>
   <si>
     <t xml:space="preserve">fax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">image</t>
   </si>
   <si>
     <t xml:space="preserve">is_company</t>
@@ -2673,10 +2691,10 @@
   </sheetPr>
   <dimension ref="A1:AE1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="630" topLeftCell="N139" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="O1" activeCellId="0" sqref="O1"/>
-      <selection pane="bottomLeft" activeCell="T161" activeCellId="0" sqref="T161"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="630" topLeftCell="N463" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="L483" activeCellId="0" sqref="L483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9181,115 +9199,112 @@
       </c>
     </row>
     <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A423" s="1" t="s">
+      <c r="A423" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="B423" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D423" s="1" t="s">
         <v>703</v>
       </c>
-      <c r="B423" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D423" s="1" t="s">
+      <c r="G423" s="2"/>
+      <c r="L423" s="1" t="s">
         <v>704</v>
-      </c>
-      <c r="J423" s="1" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A424" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="B424" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D424" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="G424" s="2"/>
+      <c r="L424" s="1" t="s">
         <v>706</v>
-      </c>
-      <c r="B424" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C424" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D424" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="G424" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A425" s="2" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="B425" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C425" s="1" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="D425" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="G425" s="2"/>
+      <c r="L425" s="1" t="s">
         <v>708</v>
-      </c>
-      <c r="G425" s="2" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A426" s="2" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="B426" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C426" s="1" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="D426" s="1" t="s">
-        <v>699</v>
+        <v>703</v>
+      </c>
+      <c r="G426" s="2"/>
+      <c r="L426" s="1" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A427" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="B427" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D427" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="G427" s="2"/>
+      <c r="L427" s="1" t="s">
         <v>706</v>
-      </c>
-      <c r="B427" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C427" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D427" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="G427" s="2" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A428" s="2" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="B428" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C428" s="1" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="D428" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="G428" s="2"/>
+      <c r="L428" s="1" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A429" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="B429" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D429" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="J429" s="1" t="s">
         <v>712</v>
-      </c>
-    </row>
-    <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A429" s="2" t="s">
-        <v>706</v>
-      </c>
-      <c r="B429" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C429" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D429" s="1" t="s">
-        <v>709</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A430" s="2" t="s">
-        <v>706</v>
+        <v>713</v>
       </c>
       <c r="B430" s="2" t="s">
         <v>38</v>
@@ -9298,7 +9313,7 @@
         <v>147</v>
       </c>
       <c r="D430" s="1" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="G430" s="2" t="s">
         <v>173</v>
@@ -9306,7 +9321,7 @@
     </row>
     <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A431" s="2" t="s">
-        <v>706</v>
+        <v>713</v>
       </c>
       <c r="B431" s="2" t="s">
         <v>38</v>
@@ -9315,15 +9330,15 @@
         <v>147</v>
       </c>
       <c r="D431" s="1" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="G431" s="2" t="s">
-        <v>173</v>
+        <v>716</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A432" s="2" t="s">
-        <v>706</v>
+        <v>713</v>
       </c>
       <c r="B432" s="2" t="s">
         <v>38</v>
@@ -9332,12 +9347,12 @@
         <v>147</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>715</v>
+        <v>699</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A433" s="2" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="B433" s="2" t="s">
         <v>38</v>
@@ -9346,12 +9361,15 @@
         <v>147</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>699</v>
+        <v>717</v>
+      </c>
+      <c r="G433" s="2" t="s">
+        <v>718</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A434" s="2" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="B434" s="2" t="s">
         <v>38</v>
@@ -9360,15 +9378,12 @@
         <v>147</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="G434" s="2" t="s">
-        <v>173</v>
+        <v>719</v>
       </c>
     </row>
     <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A435" s="2" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="B435" s="2" t="s">
         <v>38</v>
@@ -9377,15 +9392,12 @@
         <v>147</v>
       </c>
       <c r="D435" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="G435" s="2" t="s">
-        <v>173</v>
+        <v>716</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A436" s="2" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="B436" s="2" t="s">
         <v>38</v>
@@ -9394,457 +9406,481 @@
         <v>147</v>
       </c>
       <c r="D436" s="1" t="s">
-        <v>709</v>
+        <v>720</v>
+      </c>
+      <c r="G436" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A437" s="2" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="B437" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="C437" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="D437" s="1" t="s">
-        <v>718</v>
+        <v>721</v>
+      </c>
+      <c r="G437" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A438" s="2" t="s">
-        <v>719</v>
+        <v>713</v>
       </c>
       <c r="B438" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G438" s="2"/>
-      <c r="H438" s="1" t="s">
-        <v>720</v>
-      </c>
-      <c r="J438" s="1" t="s">
-        <v>721</v>
+        <v>38</v>
+      </c>
+      <c r="C438" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D438" s="1" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A439" s="2" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="B439" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G439" s="2"/>
-      <c r="H439" s="1" t="s">
-        <v>722</v>
-      </c>
-      <c r="J439" s="1" t="s">
-        <v>723</v>
+        <v>38</v>
+      </c>
+      <c r="C439" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D439" s="1" t="s">
+        <v>699</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A440" s="2" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="B440" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G440" s="2"/>
-      <c r="H440" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="J440" s="1" t="s">
-        <v>725</v>
+        <v>38</v>
+      </c>
+      <c r="C440" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D440" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="G440" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A441" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="B441" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C441" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D441" s="1" t="s">
         <v>719</v>
       </c>
-      <c r="B441" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G441" s="2"/>
-      <c r="H441" s="1" t="s">
-        <v>726</v>
-      </c>
-      <c r="J441" s="1" t="s">
-        <v>727</v>
+      <c r="G441" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A442" s="2" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="B442" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G442" s="2"/>
-      <c r="H442" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="J442" s="1" t="s">
-        <v>729</v>
+        <v>38</v>
+      </c>
+      <c r="C442" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D442" s="1" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A443" s="2" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="B443" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C443" s="1" t="s">
-        <v>731</v>
+        <v>32</v>
       </c>
       <c r="D443" s="1" t="s">
-        <v>732</v>
+        <v>725</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A444" s="2" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="B444" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C444" s="1" t="s">
-        <v>733</v>
-      </c>
-      <c r="D444" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="E444" s="2" t="s">
-        <v>735</v>
-      </c>
-      <c r="G444" s="2" t="s">
-        <v>736</v>
+        <v>32</v>
+      </c>
+      <c r="G444" s="2"/>
+      <c r="H444" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="J444" s="1" t="s">
+        <v>728</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A445" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="B445" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G445" s="2"/>
+      <c r="H445" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="J445" s="1" t="s">
         <v>730</v>
-      </c>
-      <c r="B445" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C445" s="1" t="s">
-        <v>737</v>
-      </c>
-      <c r="D445" s="1" t="s">
-        <v>738</v>
-      </c>
-      <c r="E445" s="2" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A446" s="2" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="B446" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C446" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="D446" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="G446" s="2" t="s">
-        <v>742</v>
+        <v>32</v>
+      </c>
+      <c r="G446" s="2"/>
+      <c r="H446" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="J446" s="1" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A447" s="2" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="B447" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C447" s="1" t="s">
-        <v>743</v>
-      </c>
-      <c r="D447" s="1" t="s">
-        <v>744</v>
-      </c>
-      <c r="F447" s="1" t="s">
-        <v>745</v>
+        <v>32</v>
+      </c>
+      <c r="G447" s="2"/>
+      <c r="H447" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="J447" s="1" t="s">
+        <v>734</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A448" s="2" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="B448" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C448" s="1" t="s">
-        <v>746</v>
-      </c>
-      <c r="D448" s="1" t="s">
-        <v>747</v>
-      </c>
-      <c r="F448" s="1" t="s">
-        <v>748</v>
+        <v>32</v>
+      </c>
+      <c r="G448" s="2"/>
+      <c r="H448" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="J448" s="1" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A449" s="2" t="s">
-        <v>730</v>
+        <v>737</v>
       </c>
       <c r="B449" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C449" s="1" t="s">
-        <v>749</v>
+        <v>738</v>
       </c>
       <c r="D449" s="1" t="s">
-        <v>750</v>
-      </c>
-      <c r="H449" s="1" t="s">
-        <v>751</v>
+        <v>739</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A450" s="2" t="s">
-        <v>730</v>
+        <v>737</v>
       </c>
       <c r="B450" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C450" s="1" t="s">
-        <v>752</v>
+        <v>740</v>
       </c>
       <c r="D450" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="F450" s="1" t="s">
-        <v>748</v>
+        <v>741</v>
+      </c>
+      <c r="E450" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="G450" s="2" t="s">
+        <v>743</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A451" s="2" t="s">
-        <v>730</v>
+        <v>737</v>
       </c>
       <c r="B451" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C451" s="1" t="s">
-        <v>754</v>
+        <v>744</v>
       </c>
       <c r="D451" s="1" t="s">
-        <v>734</v>
+        <v>745</v>
+      </c>
+      <c r="E451" s="2" t="s">
+        <v>746</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A452" s="2" t="s">
-        <v>730</v>
+        <v>737</v>
       </c>
       <c r="B452" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C452" s="1" t="s">
-        <v>755</v>
+        <v>747</v>
       </c>
       <c r="D452" s="1" t="s">
-        <v>756</v>
-      </c>
-      <c r="E452" s="2" t="s">
-        <v>757</v>
+        <v>748</v>
+      </c>
+      <c r="G452" s="2" t="s">
+        <v>749</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A453" s="2" t="s">
-        <v>730</v>
+        <v>737</v>
       </c>
       <c r="B453" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C453" s="1" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
       <c r="D453" s="1" t="s">
-        <v>759</v>
-      </c>
-      <c r="E453" s="2" t="s">
-        <v>760</v>
+        <v>751</v>
+      </c>
+      <c r="F453" s="1" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A454" s="2" t="s">
-        <v>730</v>
+        <v>737</v>
       </c>
       <c r="B454" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C454" s="1" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
       <c r="D454" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="G454" s="2" t="s">
-        <v>763</v>
+        <v>754</v>
+      </c>
+      <c r="F454" s="1" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A455" s="2" t="s">
-        <v>730</v>
+        <v>737</v>
       </c>
       <c r="B455" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C455" s="1" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="D455" s="1" t="s">
-        <v>765</v>
-      </c>
-      <c r="E455" s="2" t="s">
-        <v>766</v>
+        <v>757</v>
+      </c>
+      <c r="H455" s="1" t="s">
+        <v>758</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A456" s="2" t="s">
-        <v>730</v>
+        <v>737</v>
       </c>
       <c r="B456" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C456" s="1" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="D456" s="1" t="s">
-        <v>768</v>
-      </c>
-      <c r="E456" s="2" t="s">
-        <v>769</v>
+        <v>760</v>
+      </c>
+      <c r="F456" s="1" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A457" s="2" t="s">
-        <v>730</v>
+        <v>737</v>
       </c>
       <c r="B457" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C457" s="1" t="s">
-        <v>770</v>
+        <v>761</v>
       </c>
       <c r="D457" s="1" t="s">
-        <v>771</v>
-      </c>
-      <c r="E457" s="2" t="s">
-        <v>772</v>
-      </c>
-      <c r="H457" s="1" t="s">
-        <v>773</v>
+        <v>741</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A458" s="2" t="s">
-        <v>730</v>
+        <v>737</v>
       </c>
       <c r="B458" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C458" s="1" t="s">
-        <v>774</v>
+        <v>762</v>
       </c>
       <c r="D458" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="F458" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="H458" s="1" t="s">
-        <v>776</v>
+        <v>763</v>
+      </c>
+      <c r="E458" s="2" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A459" s="2" t="s">
-        <v>730</v>
+        <v>737</v>
       </c>
       <c r="B459" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C459" s="1" t="s">
-        <v>777</v>
+        <v>765</v>
       </c>
       <c r="D459" s="1" t="s">
-        <v>778</v>
+        <v>766</v>
       </c>
       <c r="E459" s="2" t="s">
-        <v>779</v>
+        <v>767</v>
       </c>
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A460" s="2" t="s">
-        <v>178</v>
+        <v>737</v>
       </c>
       <c r="B460" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E460" s="2" t="s">
-        <v>780</v>
+        <v>2</v>
+      </c>
+      <c r="C460" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="D460" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="G460" s="2" t="s">
+        <v>770</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A461" s="2" t="s">
-        <v>178</v>
+        <v>737</v>
       </c>
       <c r="B461" s="2" t="s">
-        <v>32</v>
+        <v>2</v>
+      </c>
+      <c r="C461" s="1" t="s">
+        <v>771</v>
       </c>
       <c r="D461" s="1" t="s">
-        <v>781</v>
-      </c>
-      <c r="G461" s="2" t="s">
-        <v>782</v>
+        <v>772</v>
+      </c>
+      <c r="E461" s="2" t="s">
+        <v>773</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A462" s="2" t="s">
-        <v>178</v>
+        <v>737</v>
       </c>
       <c r="B462" s="2" t="s">
-        <v>32</v>
+        <v>2</v>
+      </c>
+      <c r="C462" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="D462" s="1" t="s">
+        <v>775</v>
       </c>
       <c r="E462" s="2" t="s">
-        <v>783</v>
+        <v>776</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A463" s="2" t="s">
-        <v>178</v>
+        <v>737</v>
       </c>
       <c r="B463" s="2" t="s">
-        <v>32</v>
+        <v>2</v>
+      </c>
+      <c r="C463" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="D463" s="1" t="s">
+        <v>778</v>
       </c>
       <c r="E463" s="2" t="s">
-        <v>784</v>
+        <v>779</v>
+      </c>
+      <c r="H463" s="1" t="s">
+        <v>780</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A464" s="2" t="s">
-        <v>178</v>
+        <v>737</v>
       </c>
       <c r="B464" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E464" s="2" t="s">
-        <v>785</v>
+        <v>2</v>
+      </c>
+      <c r="C464" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="D464" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="F464" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="H464" s="1" t="s">
+        <v>783</v>
       </c>
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A465" s="2" t="s">
-        <v>178</v>
+        <v>737</v>
       </c>
       <c r="B465" s="2" t="s">
-        <v>32</v>
+        <v>2</v>
+      </c>
+      <c r="C465" s="1" t="s">
+        <v>784</v>
       </c>
       <c r="D465" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="E465" s="2" t="s">
         <v>786</v>
-      </c>
-      <c r="G465" s="2" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9854,11 +9890,8 @@
       <c r="B466" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D466" s="1" t="s">
-        <v>788</v>
-      </c>
-      <c r="G466" s="2" t="s">
-        <v>789</v>
+      <c r="E466" s="2" t="s">
+        <v>787</v>
       </c>
     </row>
     <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9868,8 +9901,11 @@
       <c r="B467" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E467" s="2" t="s">
-        <v>790</v>
+      <c r="D467" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="G467" s="2" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9880,7 +9916,7 @@
         <v>32</v>
       </c>
       <c r="E468" s="2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9891,7 +9927,7 @@
         <v>32</v>
       </c>
       <c r="E469" s="2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9902,10 +9938,10 @@
         <v>32</v>
       </c>
       <c r="D470" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="G470" s="2" t="s">
         <v>793</v>
-      </c>
-      <c r="G470" s="2" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9915,8 +9951,11 @@
       <c r="B471" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E471" s="2" t="s">
-        <v>1</v>
+      <c r="D471" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="G471" s="2" t="s">
+        <v>795</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9927,270 +9966,249 @@
         <v>32</v>
       </c>
       <c r="E472" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A473" s="1" t="s">
+      <c r="A473" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B473" s="1" t="s">
+      <c r="B473" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D473" s="1" t="s">
-        <v>796</v>
-      </c>
-      <c r="I473" s="1" t="s">
-        <v>96</v>
+      <c r="E473" s="2" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A474" s="1" t="s">
+      <c r="A474" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B474" s="1" t="s">
+      <c r="B474" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D474" s="1" t="s">
-        <v>797</v>
-      </c>
-      <c r="J474" s="1" t="s">
+      <c r="E474" s="2" t="s">
         <v>798</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A475" s="1" t="s">
+      <c r="A475" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B475" s="1" t="s">
+      <c r="B475" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D475" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="J475" s="1" t="s">
-        <v>96</v>
+      <c r="G475" s="2" t="s">
+        <v>800</v>
       </c>
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A476" s="2" t="s">
-        <v>800</v>
+        <v>178</v>
       </c>
       <c r="B476" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D476" s="1" t="s">
-        <v>801</v>
-      </c>
       <c r="E476" s="2" t="s">
-        <v>802</v>
+        <v>1</v>
       </c>
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A477" s="2" t="s">
-        <v>800</v>
+        <v>178</v>
       </c>
       <c r="B477" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D477" s="1" t="s">
+      <c r="E477" s="2" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A478" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B478" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D478" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="I478" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A479" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B479" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D479" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="E477" s="2" t="s">
+      <c r="J479" s="1" t="s">
         <v>804</v>
       </c>
     </row>
-    <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A478" s="2" t="s">
-        <v>800</v>
-      </c>
-      <c r="B478" s="2" t="s">
+    <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A480" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B480" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E478" s="2" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A479" s="2" t="s">
-        <v>800</v>
-      </c>
-      <c r="B479" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E479" s="2" t="s">
+      <c r="D480" s="1" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A480" s="2" t="s">
-        <v>800</v>
-      </c>
-      <c r="B480" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D480" s="1" t="s">
-        <v>806</v>
-      </c>
-      <c r="E480" s="2" t="s">
-        <v>807</v>
+      <c r="J480" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A481" s="2" t="s">
-        <v>808</v>
+        <v>178</v>
       </c>
       <c r="B481" s="2" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
       <c r="D481" s="1" t="s">
-        <v>809</v>
-      </c>
-      <c r="G481" s="2" t="s">
-        <v>810</v>
+        <v>703</v>
+      </c>
+      <c r="G481" s="2"/>
+      <c r="L481" s="1" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A482" s="2" t="s">
-        <v>808</v>
+        <v>178</v>
       </c>
       <c r="B482" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D482" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H482" s="1" t="s">
-        <v>112</v>
+        <v>705</v>
+      </c>
+      <c r="G482" s="2"/>
+      <c r="L482" s="1" t="s">
+        <v>706</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A483" s="2" t="s">
-        <v>808</v>
+        <v>178</v>
       </c>
       <c r="B483" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C483" s="1" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="D483" s="1" t="s">
-        <v>699</v>
+        <v>707</v>
+      </c>
+      <c r="G483" s="2"/>
+      <c r="L483" s="1" t="s">
+        <v>708</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A484" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="B484" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D484" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="E484" s="2" t="s">
         <v>808</v>
-      </c>
-      <c r="B484" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C484" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D484" s="1" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A485" s="2" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B485" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C485" s="1" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="D485" s="1" t="s">
-        <v>709</v>
+        <v>809</v>
+      </c>
+      <c r="E485" s="2" t="s">
+        <v>810</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A486" s="2" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B486" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C486" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D486" s="1" t="s">
-        <v>811</v>
-      </c>
-      <c r="G486" s="2" t="s">
-        <v>126</v>
+        <v>32</v>
+      </c>
+      <c r="E486" s="2" t="s">
+        <v>787</v>
       </c>
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A487" s="2" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B487" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C487" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D487" s="1" t="s">
-        <v>812</v>
-      </c>
-      <c r="G487" s="2" t="s">
-        <v>126</v>
+        <v>32</v>
+      </c>
+      <c r="E487" s="2" t="s">
+        <v>811</v>
       </c>
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A488" s="2" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B488" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C488" s="1" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="D488" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="E488" s="2" t="s">
         <v>813</v>
-      </c>
-      <c r="G488" s="2" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A489" s="2" t="s">
-        <v>808</v>
+        <v>814</v>
       </c>
       <c r="B489" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C489" s="1" t="s">
-        <v>147</v>
+        <v>90</v>
       </c>
       <c r="D489" s="1" t="s">
-        <v>715</v>
+        <v>815</v>
+      </c>
+      <c r="G489" s="2" t="s">
+        <v>816</v>
       </c>
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A490" s="2" t="s">
-        <v>808</v>
+        <v>814</v>
       </c>
       <c r="B490" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C490" s="1" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="D490" s="1" t="s">
-        <v>814</v>
-      </c>
-      <c r="G490" s="2" t="s">
-        <v>126</v>
+        <v>111</v>
+      </c>
+      <c r="H490" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A491" s="2" t="s">
-        <v>808</v>
+        <v>814</v>
       </c>
       <c r="B491" s="2" t="s">
         <v>38</v>
@@ -10199,26 +10217,26 @@
         <v>147</v>
       </c>
       <c r="D491" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="G491" s="2" t="s">
-        <v>126</v>
+        <v>699</v>
       </c>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A492" s="2" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B492" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="C492" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="D492" s="1" t="s">
-        <v>817</v>
+        <v>719</v>
       </c>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A493" s="2" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B493" s="2" t="s">
         <v>38</v>
@@ -10227,15 +10245,12 @@
         <v>147</v>
       </c>
       <c r="D493" s="1" t="s">
-        <v>818</v>
-      </c>
-      <c r="H493" s="1" t="s">
-        <v>709</v>
+        <v>716</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A494" s="2" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B494" s="2" t="s">
         <v>38</v>
@@ -10244,15 +10259,15 @@
         <v>147</v>
       </c>
       <c r="D494" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="H494" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="G494" s="2" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A495" s="2" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B495" s="2" t="s">
         <v>38</v>
@@ -10261,12 +10276,15 @@
         <v>147</v>
       </c>
       <c r="D495" s="1" t="s">
-        <v>699</v>
+        <v>818</v>
+      </c>
+      <c r="G495" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A496" s="2" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B496" s="2" t="s">
         <v>38</v>
@@ -10275,12 +10293,15 @@
         <v>147</v>
       </c>
       <c r="D496" s="1" t="s">
-        <v>712</v>
+        <v>819</v>
+      </c>
+      <c r="G496" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A497" s="2" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B497" s="2" t="s">
         <v>38</v>
@@ -10289,29 +10310,41 @@
         <v>147</v>
       </c>
       <c r="D497" s="1" t="s">
-        <v>709</v>
+        <v>722</v>
       </c>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A498" s="2" t="s">
-        <v>819</v>
+        <v>814</v>
       </c>
       <c r="B498" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="C498" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="D498" s="1" t="s">
         <v>820</v>
       </c>
+      <c r="G498" s="2" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A499" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="B499" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C499" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D499" s="1" t="s">
         <v>821</v>
       </c>
-      <c r="B499" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D499" s="1" t="s">
-        <v>122</v>
+      <c r="G499" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10322,12 +10355,122 @@
         <v>32</v>
       </c>
       <c r="D500" s="1" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A501" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="B501" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C501" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D501" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="H501" s="1" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A502" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="B502" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C502" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D502" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="H502" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A503" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="B503" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C503" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D503" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A504" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="B504" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C504" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D504" s="1" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A505" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="B505" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C505" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D505" s="1" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A506" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="B506" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D506" s="1" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A507" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="B507" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D507" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A508" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="B508" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D508" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="G500" s="2" t="s">
-        <v>823</v>
-      </c>
-    </row>
+      <c r="G508" s="2" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>